<commit_message>
completed Expense section of P&L report
</commit_message>
<xml_diff>
--- a/AccountReportApp/Data/Demo_Accounts.xlsx
+++ b/AccountReportApp/Data/Demo_Accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AccountReports\AccountReportApp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C895E42-9836-4D21-96D0-E68163CBD0C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{529FA4BD-8494-41D8-B8B6-3BED6EA71C97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25380" yWindow="2175" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{DB0C3B61-0213-4CC9-A985-0DFF80DDBF0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DB0C3B61-0213-4CC9-A985-0DFF80DDBF0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="134">
   <si>
     <t>Client</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>Contract</t>
-  </si>
-  <si>
     <t>Payroll Taxes</t>
   </si>
   <si>
@@ -122,18 +119,9 @@
     <t>Continuing Education</t>
   </si>
   <si>
-    <t>Bank service charge</t>
-  </si>
-  <si>
-    <t>Professional Fee</t>
-  </si>
-  <si>
     <t>Insurance</t>
   </si>
   <si>
-    <t>Payroll Services</t>
-  </si>
-  <si>
     <t>InvNum</t>
   </si>
   <si>
@@ -236,9 +224,6 @@
     <t>email addresses</t>
   </si>
   <si>
-    <t>Member draw</t>
-  </si>
-  <si>
     <t>Web stuff</t>
   </si>
   <si>
@@ -413,9 +398,6 @@
     <t>ExpClass</t>
   </si>
   <si>
-    <t>Service Fees</t>
-  </si>
-  <si>
     <t>Office</t>
   </si>
   <si>
@@ -429,6 +411,33 @@
   </si>
   <si>
     <t>Paypal</t>
+  </si>
+  <si>
+    <t>Bank Fees</t>
+  </si>
+  <si>
+    <t>Professional Services</t>
+  </si>
+  <si>
+    <t>annual tax prep</t>
+  </si>
+  <si>
+    <t>Bank Service Charge</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Payroll</t>
+  </si>
+  <si>
+    <t>Marketting</t>
   </si>
 </sst>
 </file>
@@ -831,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
@@ -863,10 +872,10 @@
         <v>44197</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>1001</v>
@@ -898,10 +907,10 @@
         <v>44198</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>1002</v>
@@ -933,10 +942,10 @@
         <v>44199</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>1003</v>
@@ -968,10 +977,10 @@
         <v>44200</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D5">
         <v>1004</v>
@@ -1003,10 +1012,10 @@
         <v>44201</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>1005</v>
@@ -1038,10 +1047,10 @@
         <v>44202</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>1006</v>
@@ -1073,10 +1082,10 @@
         <v>44203</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>1007</v>
@@ -1093,10 +1102,10 @@
         <v>44204</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>1008</v>
@@ -1113,10 +1122,10 @@
         <v>44205</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>1009</v>
@@ -1134,10 +1143,10 @@
         <v>44206</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>1010</v>
@@ -1174,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0524AE-04CC-4834-B839-8A5DF144FBEE}">
-  <dimension ref="A1:XFC53"/>
+  <dimension ref="A1:XFA53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,63 +1201,61 @@
     <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16383" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="19.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16381" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44208</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="H2">
         <v>260</v>
@@ -1256,29 +1263,29 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44209</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H3">
         <v>12</v>
@@ -1286,29 +1293,29 @@
       <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44250</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -1316,29 +1323,29 @@
       <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44197</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -1346,29 +1353,29 @@
       <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44197</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H6">
         <v>20</v>
@@ -1376,29 +1383,29 @@
       <c r="I6" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44197</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -1406,29 +1413,29 @@
       <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44199</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H8">
         <v>100</v>
@@ -1436,29 +1443,29 @@
       <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44204</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -1466,29 +1473,29 @@
       <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44206</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H10">
         <v>75</v>
@@ -1496,29 +1503,29 @@
       <c r="I10" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44208</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H11">
         <v>30</v>
@@ -1526,29 +1533,29 @@
       <c r="I11" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44216</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H12">
         <v>4</v>
@@ -1556,29 +1563,29 @@
       <c r="I12" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44217</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H13">
         <v>65</v>
@@ -1586,29 +1593,29 @@
       <c r="I13" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44226</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1616,29 +1623,29 @@
       <c r="I14" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44228</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H15">
         <v>15</v>
@@ -1646,30 +1653,29 @@
       <c r="I15" t="s">
         <v>17</v>
       </c>
-      <c r="L15"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44228</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H16">
         <v>20</v>
@@ -1677,30 +1683,29 @@
       <c r="I16" t="s">
         <v>17</v>
       </c>
-      <c r="L16"/>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44229</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -1708,30 +1713,29 @@
       <c r="I17" t="s">
         <v>17</v>
       </c>
-      <c r="L17"/>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44230</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H18">
         <v>100</v>
@@ -1739,30 +1743,29 @@
       <c r="I18" t="s">
         <v>17</v>
       </c>
-      <c r="L18"/>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44235</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -1770,30 +1773,30 @@
       <c r="I19" t="s">
         <v>17</v>
       </c>
+      <c r="K19"/>
       <c r="L19"/>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44239</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H20">
         <v>30</v>
@@ -1801,30 +1804,30 @@
       <c r="I20" t="s">
         <v>17</v>
       </c>
+      <c r="K20"/>
       <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44246</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H21">
         <v>12</v>
@@ -1832,30 +1835,30 @@
       <c r="I21" t="s">
         <v>17</v>
       </c>
+      <c r="K21"/>
       <c r="L21"/>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44247</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H22">
         <v>50</v>
@@ -1863,30 +1866,30 @@
       <c r="I22" t="s">
         <v>17</v>
       </c>
+      <c r="K22"/>
       <c r="L22"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44248</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>4</v>
@@ -1894,30 +1897,30 @@
       <c r="I23" t="s">
         <v>17</v>
       </c>
+      <c r="K23"/>
       <c r="L23"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44255</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1925,30 +1928,30 @@
       <c r="I24" t="s">
         <v>17</v>
       </c>
+      <c r="K24"/>
       <c r="L24"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44216</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H25">
         <v>30</v>
@@ -1956,30 +1959,30 @@
       <c r="I25" t="s">
         <v>17</v>
       </c>
+      <c r="K25"/>
       <c r="L25"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44219</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H26">
         <v>40</v>
@@ -1987,30 +1990,30 @@
       <c r="I26" t="s">
         <v>17</v>
       </c>
+      <c r="K26"/>
       <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44223</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F27" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H27">
         <v>2000</v>
@@ -2018,30 +2021,30 @@
       <c r="I27" t="s">
         <v>17</v>
       </c>
+      <c r="K27"/>
       <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44249</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H28">
         <v>220</v>
@@ -2049,30 +2052,30 @@
       <c r="I28" t="s">
         <v>17</v>
       </c>
+      <c r="K28"/>
       <c r="L28"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44200</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H29">
         <v>200</v>
@@ -2080,30 +2083,30 @@
       <c r="I29" t="s">
         <v>11</v>
       </c>
+      <c r="K29"/>
       <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44208</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H30">
         <v>1000</v>
@@ -2111,30 +2114,30 @@
       <c r="I30" t="s">
         <v>17</v>
       </c>
+      <c r="K30"/>
       <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44209</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H31">
         <v>3000</v>
@@ -2142,30 +2145,30 @@
       <c r="I31" t="s">
         <v>17</v>
       </c>
+      <c r="K31"/>
       <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44211</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="G32" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H32">
         <v>800</v>
@@ -2173,30 +2176,30 @@
       <c r="I32" t="s">
         <v>17</v>
       </c>
+      <c r="K32"/>
       <c r="L32"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44225</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H33">
         <v>2000</v>
@@ -2204,29 +2207,30 @@
       <c r="I33" t="s">
         <v>17</v>
       </c>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K33"/>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44237</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F34" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="G34" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H34">
         <v>700</v>
@@ -2234,29 +2238,30 @@
       <c r="I34" t="s">
         <v>17</v>
       </c>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K34"/>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44202</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F35" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="G35" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H35">
         <v>100</v>
@@ -2264,29 +2269,30 @@
       <c r="I35" t="s">
         <v>17</v>
       </c>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K35"/>
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44216</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="G36" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H36">
         <v>35</v>
@@ -2294,29 +2300,30 @@
       <c r="I36" t="s">
         <v>17</v>
       </c>
-      <c r="M36" s="4"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K36"/>
+      <c r="L36"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44230</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="G37" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H37">
         <v>35</v>
@@ -2324,29 +2331,29 @@
       <c r="I37" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>44244</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="G38" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H38">
         <v>35</v>
@@ -2354,29 +2361,29 @@
       <c r="I38" t="s">
         <v>17</v>
       </c>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>44202</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H39">
         <v>50</v>
@@ -2384,29 +2391,29 @@
       <c r="I39" t="s">
         <v>17</v>
       </c>
-      <c r="M39" s="4"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>44216</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H40">
         <v>100</v>
@@ -2414,29 +2421,29 @@
       <c r="I40" t="s">
         <v>17</v>
       </c>
-      <c r="M40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>44230</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H41">
         <v>150</v>
@@ -2444,29 +2451,29 @@
       <c r="I41" t="s">
         <v>17</v>
       </c>
-      <c r="M41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>44244</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G42" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H42">
         <v>90</v>
@@ -2474,29 +2481,29 @@
       <c r="I42" t="s">
         <v>17</v>
       </c>
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>44218</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G43" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H43">
         <v>40</v>
@@ -2504,29 +2511,29 @@
       <c r="I43" t="s">
         <v>17</v>
       </c>
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44217</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F44" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="G44" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H44">
         <v>40</v>
@@ -2534,29 +2541,29 @@
       <c r="I44" t="s">
         <v>17</v>
       </c>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44248</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="F45" t="s">
         <v>21</v>
       </c>
       <c r="G45" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H45">
         <v>500</v>
@@ -2564,29 +2571,29 @@
       <c r="I45" t="s">
         <v>17</v>
       </c>
-      <c r="M45" s="4"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44218</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="F46" t="s">
         <v>21</v>
       </c>
       <c r="G46" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H46">
         <v>500</v>
@@ -2594,29 +2601,29 @@
       <c r="I46" t="s">
         <v>17</v>
       </c>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>44202</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F47" t="s">
         <v>23</v>
       </c>
       <c r="G47" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H47">
         <v>500</v>
@@ -2624,29 +2631,29 @@
       <c r="I47" t="s">
         <v>17</v>
       </c>
-      <c r="M47" s="4"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>44216</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F48" t="s">
         <v>23</v>
       </c>
       <c r="G48" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H48">
         <v>1000</v>
@@ -2654,29 +2661,29 @@
       <c r="I48" t="s">
         <v>17</v>
       </c>
-      <c r="M48" s="4"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>44230</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
         <v>23</v>
       </c>
       <c r="G49" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H49">
         <v>1500</v>
@@ -2684,29 +2691,29 @@
       <c r="I49" t="s">
         <v>17</v>
       </c>
-      <c r="M49" s="4"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>44244</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F50" t="s">
         <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H50">
         <v>900</v>
@@ -2714,29 +2721,29 @@
       <c r="I50" t="s">
         <v>17</v>
       </c>
-      <c r="M50" s="4"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>44211</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F51" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G51" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H51">
         <v>600</v>
@@ -2744,29 +2751,29 @@
       <c r="I51" t="s">
         <v>11</v>
       </c>
-      <c r="M51" s="4"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>44198</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F52" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G52" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H52">
         <v>250</v>
@@ -2774,29 +2781,29 @@
       <c r="I52" t="s">
         <v>11</v>
       </c>
-      <c r="M52" s="4"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>44212</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="F53" t="s">
         <v>21</v>
       </c>
       <c r="G53" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H53">
         <v>2000</v>
@@ -2804,19 +2811,20 @@
       <c r="I53" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="4"/>
+      <c r="K53" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K50">
     <sortCondition ref="J2:J50"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G54:H160 F2:F53" xr:uid="{D5E8F5CA-18C4-4246-8E3E-7E6AF8FCFB1C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G54:H160" xr:uid="{D5E8F5CA-18C4-4246-8E3E-7E6AF8FCFB1C}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2850,7 +2858,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -2870,25 +2878,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2896,25 +2904,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2922,22 +2930,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2945,22 +2953,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2968,22 +2976,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2991,22 +2999,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3014,22 +3022,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -3037,22 +3045,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
demo data value correction
</commit_message>
<xml_diff>
--- a/AccountReportApp/Data/Demo_Accounts.xlsx
+++ b/AccountReportApp/Data/Demo_Accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AccountReports\AccountReportApp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{529FA4BD-8494-41D8-B8B6-3BED6EA71C97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48FCB57-554D-4E40-98E8-0E50FDBD651C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DB0C3B61-0213-4CC9-A985-0DFF80DDBF0B}"/>
   </bookViews>
@@ -233,9 +233,6 @@
     <t>Various Fees</t>
   </si>
   <si>
-    <t>Payroll services</t>
-  </si>
-  <si>
     <t>Employee salary direct deposit</t>
   </si>
   <si>
@@ -438,6 +435,9 @@
   </si>
   <si>
     <t>Marketting</t>
+  </si>
+  <si>
+    <t>Payroll services fee</t>
   </si>
 </sst>
 </file>
@@ -980,7 +980,7 @@
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5">
         <v>1004</v>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0524AE-04CC-4834-B839-8A5DF144FBEE}">
   <dimension ref="A1:XFA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1207,31 +1207,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="K1" s="4"/>
     </row>
@@ -1240,22 +1240,22 @@
         <v>44208</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
         <v>126</v>
-      </c>
-      <c r="F2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" t="s">
-        <v>127</v>
       </c>
       <c r="H2">
         <v>260</v>
@@ -1270,19 +1270,19 @@
         <v>44209</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G3" t="s">
         <v>64</v>
@@ -1300,19 +1300,19 @@
         <v>44250</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G4" t="s">
         <v>64</v>
@@ -1330,22 +1330,22 @@
         <v>44197</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -1360,22 +1360,22 @@
         <v>44197</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H6">
         <v>20</v>
@@ -1390,22 +1390,22 @@
         <v>44197</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -1420,22 +1420,22 @@
         <v>44199</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8">
         <v>100</v>
@@ -1450,22 +1450,22 @@
         <v>44204</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -1480,22 +1480,22 @@
         <v>44206</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10">
         <v>75</v>
@@ -1510,16 +1510,16 @@
         <v>44208</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -1540,22 +1540,22 @@
         <v>44216</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12">
         <v>4</v>
@@ -1570,22 +1570,22 @@
         <v>44217</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H13">
         <v>65</v>
@@ -1600,22 +1600,22 @@
         <v>44226</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1630,22 +1630,22 @@
         <v>44228</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15">
         <v>15</v>
@@ -1660,22 +1660,22 @@
         <v>44228</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16">
         <v>20</v>
@@ -1690,22 +1690,22 @@
         <v>44229</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -1720,22 +1720,22 @@
         <v>44230</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H18">
         <v>100</v>
@@ -1750,22 +1750,22 @@
         <v>44235</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -1781,16 +1781,16 @@
         <v>44239</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
@@ -1812,22 +1812,22 @@
         <v>44246</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21">
         <v>12</v>
@@ -1843,22 +1843,22 @@
         <v>44247</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22">
         <v>50</v>
@@ -1874,22 +1874,22 @@
         <v>44248</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H23">
         <v>4</v>
@@ -1905,22 +1905,22 @@
         <v>44255</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1936,22 +1936,22 @@
         <v>44216</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F25" t="s">
         <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H25">
         <v>30</v>
@@ -1967,22 +1967,22 @@
         <v>44219</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s">
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H26">
         <v>40</v>
@@ -1998,22 +1998,22 @@
         <v>44223</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="s">
         <v>80</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" t="s">
-        <v>81</v>
       </c>
       <c r="H27">
         <v>2000</v>
@@ -2029,16 +2029,16 @@
         <v>44249</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" t="s">
         <v>27</v>
@@ -2060,22 +2060,22 @@
         <v>44200</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H29">
         <v>200</v>
@@ -2091,22 +2091,22 @@
         <v>44208</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H30">
         <v>1000</v>
@@ -2122,25 +2122,25 @@
         <v>44209</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H31">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="I31" t="s">
         <v>17</v>
@@ -2153,22 +2153,22 @@
         <v>44211</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H32">
         <v>800</v>
@@ -2184,22 +2184,22 @@
         <v>44225</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33">
         <v>2000</v>
@@ -2215,22 +2215,22 @@
         <v>44237</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H34">
         <v>700</v>
@@ -2246,22 +2246,22 @@
         <v>44202</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G35" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="H35">
         <v>100</v>
@@ -2277,22 +2277,22 @@
         <v>44216</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G36" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="H36">
         <v>35</v>
@@ -2308,22 +2308,22 @@
         <v>44230</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G37" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="H37">
         <v>35</v>
@@ -2338,22 +2338,22 @@
         <v>44244</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G38" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="H38">
         <v>35</v>
@@ -2368,22 +2368,22 @@
         <v>44202</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F39" t="s">
         <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H39">
         <v>50</v>
@@ -2398,22 +2398,22 @@
         <v>44216</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F40" t="s">
         <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H40">
         <v>100</v>
@@ -2428,22 +2428,22 @@
         <v>44230</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F41" t="s">
         <v>24</v>
       </c>
       <c r="G41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H41">
         <v>150</v>
@@ -2458,22 +2458,22 @@
         <v>44244</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F42" t="s">
         <v>24</v>
       </c>
       <c r="G42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H42">
         <v>90</v>
@@ -2488,22 +2488,22 @@
         <v>44218</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F43" t="s">
         <v>25</v>
       </c>
       <c r="G43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H43">
         <v>40</v>
@@ -2518,22 +2518,22 @@
         <v>44217</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H44">
         <v>40</v>
@@ -2548,22 +2548,22 @@
         <v>44248</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F45" t="s">
         <v>21</v>
       </c>
       <c r="G45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H45">
         <v>500</v>
@@ -2578,22 +2578,22 @@
         <v>44218</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F46" t="s">
         <v>21</v>
       </c>
       <c r="G46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H46">
         <v>500</v>
@@ -2608,22 +2608,22 @@
         <v>44202</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F47" t="s">
         <v>23</v>
       </c>
       <c r="G47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H47">
         <v>500</v>
@@ -2638,22 +2638,22 @@
         <v>44216</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F48" t="s">
         <v>23</v>
       </c>
       <c r="G48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H48">
         <v>1000</v>
@@ -2668,22 +2668,22 @@
         <v>44230</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F49" t="s">
         <v>23</v>
       </c>
       <c r="G49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H49">
         <v>1500</v>
@@ -2698,22 +2698,22 @@
         <v>44244</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F50" t="s">
         <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H50">
         <v>900</v>
@@ -2728,22 +2728,22 @@
         <v>44211</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" t="s">
+        <v>77</v>
+      </c>
+      <c r="G51" t="s">
         <v>78</v>
-      </c>
-      <c r="F51" t="s">
-        <v>78</v>
-      </c>
-      <c r="G51" t="s">
-        <v>79</v>
       </c>
       <c r="H51">
         <v>600</v>
@@ -2758,22 +2758,22 @@
         <v>44198</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H52">
         <v>250</v>
@@ -2788,22 +2788,22 @@
         <v>44212</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F53" t="s">
         <v>21</v>
       </c>
       <c r="G53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H53">
         <v>2000</v>

</xml_diff>

<commit_message>
added IncType column to income spreadsheet and updated associated app and report code; added other income types to demo data
</commit_message>
<xml_diff>
--- a/AccountReportApp/Data/Demo_Accounts.xlsx
+++ b/AccountReportApp/Data/Demo_Accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AccountReports\AccountReportApp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48FCB57-554D-4E40-98E8-0E50FDBD651C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF127F2-ECE4-42C2-8B0D-BD1C428886C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DB0C3B61-0213-4CC9-A985-0DFF80DDBF0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB0C3B61-0213-4CC9-A985-0DFF80DDBF0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="140">
   <si>
     <t>Client</t>
   </si>
@@ -438,6 +438,24 @@
   </si>
   <si>
     <t>Payroll services fee</t>
+  </si>
+  <si>
+    <t>IncType</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Bank Interest</t>
+  </si>
+  <si>
+    <t>BigBank</t>
+  </si>
+  <si>
+    <t>Royalties</t>
+  </si>
+  <si>
+    <t>SciPublisher Inc</t>
   </si>
 </sst>
 </file>
@@ -808,376 +826,433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2391E062-DC20-4417-A025-05D9A467AE93}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44197</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1">
         <v>44227</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1000</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44198</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1002</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5000</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1">
         <v>44249</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5000</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3">
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44199</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1003</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2500</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>44249</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2500</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44200</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>123</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1004</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6000</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1">
         <v>44208</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>6000</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5">
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44201</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1005</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3000</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1">
         <v>44207</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>3000</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6">
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44202</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1006</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1000</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1">
         <v>44207</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1000</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7">
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44203</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1007</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2500</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44204</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1008</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2500</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44205</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1009</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1000</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44206</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1010</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2500</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="1"/>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="1">
+        <v>44211</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>137</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="1">
+        <v>44206</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I19 J2:J21" xr:uid="{4EF89832-E8A7-4D3F-A94E-43F08F58EB04}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8079E537-3A57-44CE-8BAF-CC60FABE2569}">
-          <x14:formula1>
-            <xm:f>Clients!$C$2:$C$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B19</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1185,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0524AE-04CC-4834-B839-8A5DF144FBEE}">
   <dimension ref="A1:XFA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2818,11 +2893,6 @@
     <sortCondition ref="J2:J50"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G54:H160" xr:uid="{D5E8F5CA-18C4-4246-8E3E-7E6AF8FCFB1C}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2833,7 +2903,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
major updates to report structure (denser summaries in main and details moved to appendix; reportng of "other income")
</commit_message>
<xml_diff>
--- a/AccountReportApp/Data/Demo_Accounts.xlsx
+++ b/AccountReportApp/Data/Demo_Accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AccountReports\AccountReportApp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF127F2-ECE4-42C2-8B0D-BD1C428886C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE22DB9-170B-47E8-88F5-669C535CFE10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB0C3B61-0213-4CC9-A985-0DFF80DDBF0B}"/>
   </bookViews>
@@ -829,7 +829,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,8 +1260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0524AE-04CC-4834-B839-8A5DF144FBEE}">
   <dimension ref="A1:XFA53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>